<commit_message>
Fix some bugs and amend the calculation of upper bounds values
</commit_message>
<xml_diff>
--- a/File/Lattice.xlsx
+++ b/File/Lattice.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6500" yWindow="8820" windowWidth="23060" windowHeight="14020" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="9520" yWindow="2200" windowWidth="23060" windowHeight="14020" tabRatio="500" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="117">
   <si>
     <t>null</t>
   </si>
@@ -558,6 +559,27 @@
   </si>
   <si>
     <t>checkSubsetsX(sofar = [49, -1], remaining = [31], limit = 49, cnt = 3472, new_sup = 0.412547, alpha = 0.05)</t>
+  </si>
+  <si>
+    <t>-1, 49, 31, 18</t>
+  </si>
+  <si>
+    <t>field20 = PENDANT/field6 = NONE/field9 = BROAD</t>
+  </si>
+  <si>
+    <t>EDIBLE/field20 = PENDANT/field6 = NONE/field9 = BROAD</t>
+  </si>
+  <si>
+    <t>field12 = ROOTED</t>
+  </si>
+  <si>
+    <t>EDIBLE/field12 = ROOTED</t>
+  </si>
+  <si>
+    <t>lift</t>
+  </si>
+  <si>
+    <t>leverage</t>
   </si>
 </sst>
 </file>
@@ -745,7 +767,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -762,9 +784,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1564,10 +1587,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1834,9 +1857,11 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="A25" s="7" t="s">
         <v>105</v>
       </c>
+      <c r="B25" s="8"/>
+      <c r="C25" s="9"/>
       <c r="E25" t="s">
         <v>108</v>
       </c>
@@ -1845,10 +1870,10 @@
       <c r="A26" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="11">
         <v>3544</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="12">
         <f>B26/$B$1</f>
         <v>0.42110266159695819</v>
       </c>
@@ -1857,33 +1882,171 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="A27" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="11">
         <v>3472</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="12">
         <f>B27/$B$1</f>
         <v>0.41254752851711024</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="A28" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="B28">
-        <f>C27/(C26*C2)</f>
+      <c r="B28" s="11">
+        <f>C27/(C26*$C$2)</f>
         <v>1.8371257388652156</v>
       </c>
+      <c r="C28" s="12"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="A29" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="B29">
-        <f>C27-C26*C2</f>
+      <c r="B29" s="14">
+        <f>C27-C26*$C$2</f>
         <v>0.18798612817880839</v>
+      </c>
+      <c r="C29" s="15"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="17" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>111</v>
+      </c>
+      <c r="B32">
+        <v>2328</v>
+      </c>
+      <c r="C32" s="12">
+        <f>B32/$B$1</f>
+        <v>0.27661596958174905</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>112</v>
+      </c>
+      <c r="B33">
+        <v>2256</v>
+      </c>
+      <c r="C33" s="12">
+        <f>B33/$B$1</f>
+        <v>0.26806083650190116</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="11">
+        <f>C33/(C32*$C$2)</f>
+        <v>1.8172262344487933</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B35" s="14">
+        <f>C33-C32*$C$2</f>
+        <v>0.12054984892075929</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1">
+        <v>8416</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2">
+        <v>4488</v>
+      </c>
+      <c r="C2">
+        <f>B2/$B$1</f>
+        <v>0.53326996197718635</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3">
+        <v>3928</v>
+      </c>
+      <c r="C3">
+        <f>B3/$B$1</f>
+        <v>0.46673003802281371</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6">
+        <v>192</v>
+      </c>
+      <c r="C6">
+        <f>B6/$B$1</f>
+        <v>2.2813688212927757E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7">
+        <v>192</v>
+      </c>
+      <c r="C7">
+        <f>B7/B1</f>
+        <v>2.2813688212927757E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9">
+        <f>C7/(C6*C2)</f>
+        <v>1.8752228163992868</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10">
+        <f>C7-C6*C2</f>
+        <v>1.0647833567060387E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Save the actual lift/leverage for 2-itemset[1-itemset + consequent]
</commit_message>
<xml_diff>
--- a/File/Lattice.xlsx
+++ b/File/Lattice.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9520" yWindow="2200" windowWidth="23060" windowHeight="14020" tabRatio="500" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="4620" yWindow="3500" windowWidth="23060" windowHeight="14020" tabRatio="500" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="129">
   <si>
     <t>null</t>
   </si>
@@ -570,16 +570,52 @@
     <t>EDIBLE/field20 = PENDANT/field6 = NONE/field9 = BROAD</t>
   </si>
   <si>
-    <t>field12 = ROOTED</t>
-  </si>
-  <si>
-    <t>EDIBLE/field12 = ROOTED</t>
-  </si>
-  <si>
-    <t>lift</t>
-  </si>
-  <si>
-    <t>leverage</t>
+    <t>field7 = FREE</t>
+  </si>
+  <si>
+    <t>EDIBLE/field7 = FREE</t>
+  </si>
+  <si>
+    <t>upper bound - leverage</t>
+  </si>
+  <si>
+    <t>field11 = TAPERING</t>
+  </si>
+  <si>
+    <t>field13 = SMOOTH</t>
+  </si>
+  <si>
+    <t>field14 = SMOOTH</t>
+  </si>
+  <si>
+    <t>EDIBLE/field11 = TAPERING</t>
+  </si>
+  <si>
+    <t>EDIBLE/field13 = SMOOTH</t>
+  </si>
+  <si>
+    <t>EDIBLE/field14 = SMOOTH</t>
+  </si>
+  <si>
+    <t>&lt;=0.5</t>
+  </si>
+  <si>
+    <t>&gt;0.5</t>
+  </si>
+  <si>
+    <t>upper bound - lift</t>
+  </si>
+  <si>
+    <t>field19 = ONE</t>
+  </si>
+  <si>
+    <t>EDIBLE/field19 = ONE</t>
+  </si>
+  <si>
+    <t>actual - leverage</t>
+  </si>
+  <si>
+    <t>actual - lift</t>
   </si>
 </sst>
 </file>
@@ -660,7 +696,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -763,11 +799,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -788,6 +904,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1967,44 +2094,53 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="8">
         <v>8416</v>
       </c>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="11">
         <v>4488</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="12">
         <f>B2/$B$1</f>
         <v>0.53326996197718635</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="14">
         <v>3928</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="15">
         <f>B3/$B$1</f>
         <v>0.46673003802281371</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2012,11 +2148,11 @@
         <v>113</v>
       </c>
       <c r="B6">
-        <v>192</v>
+        <v>8200</v>
       </c>
       <c r="C6">
         <f>B6/$B$1</f>
-        <v>2.2813688212927757E-2</v>
+        <v>0.9743346007604563</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2024,29 +2160,392 @@
         <v>114</v>
       </c>
       <c r="B7">
-        <v>192</v>
+        <v>4296</v>
       </c>
       <c r="C7">
-        <f>B7/B1</f>
-        <v>2.2813688212927757E-2</v>
+        <f>B7/$B$1</f>
+        <v>0.51045627376425851</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="B8">
+        <f>MIN(C6,$C$2) - C6 * $C$2</f>
+        <v>1.3686586476600815E-2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>115</v>
-      </c>
-      <c r="B9">
-        <f>C7/(C6*C2)</f>
-        <v>1.8752228163992868</v>
+        <v>123</v>
+      </c>
+      <c r="B9" s="1">
+        <f>MIN($C$2, 0.5) - $C$2 * 0.5</f>
+        <v>0.23336501901140683</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10">
+        <f>IF(C6 &lt;= 0.5, B8, B9)</f>
+        <v>0.23336501901140683</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" s="1">
+        <f>1/$C$2</f>
+        <v>1.8752228163992868</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>116</v>
       </c>
-      <c r="B10">
-        <f>C7-C6*C2</f>
-        <v>1.0647833567060387E-2</v>
+      <c r="B14">
+        <v>4864</v>
+      </c>
+      <c r="C14">
+        <f>B14/$B$1</f>
+        <v>0.57794676806083645</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15">
+        <v>2848</v>
+      </c>
+      <c r="C15">
+        <f>B15/$B$1</f>
+        <v>0.33840304182509506</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="B16">
+        <f>MIN(C14,$C$2) - C14 * $C$2</f>
+        <v>0.22506831094854635</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17" s="1">
+        <f>MIN($C$2, 0.5) - $C$2 * 0.5</f>
+        <v>0.23336501901140683</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>115</v>
+      </c>
+      <c r="B18">
+        <f>IF(C14 &lt;= 0.5, B16, B17)</f>
+        <v>0.23336501901140683</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>124</v>
+      </c>
+      <c r="B19" s="1">
+        <f>1/$C$2</f>
+        <v>1.8752228163992868</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>117</v>
+      </c>
+      <c r="B23">
+        <v>5316</v>
+      </c>
+      <c r="C23">
+        <f>B23/$B$1</f>
+        <v>0.63165399239543729</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>120</v>
+      </c>
+      <c r="B24">
+        <v>3780</v>
+      </c>
+      <c r="C24">
+        <f>B24/$B$1</f>
+        <v>0.44914448669201523</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="B25">
+        <f>MIN(C23,$C$2) - C23 * $C$2</f>
+        <v>0.19642786146973357</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>123</v>
+      </c>
+      <c r="B26" s="1">
+        <f>MIN($C$2, 0.5) - $C$2 * 0.5</f>
+        <v>0.23336501901140683</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>115</v>
+      </c>
+      <c r="B27">
+        <f>IF(C23 &lt;= 0.5, B25, B26)</f>
+        <v>0.23336501901140683</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28" s="1">
+        <f>1/$C$2</f>
+        <v>1.8752228163992868</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>118</v>
+      </c>
+      <c r="B31">
+        <v>5076</v>
+      </c>
+      <c r="C31">
+        <f>B31/$B$1</f>
+        <v>0.60313688212927752</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>121</v>
+      </c>
+      <c r="B32">
+        <v>3540</v>
+      </c>
+      <c r="C32">
+        <f>B32/$B$1</f>
+        <v>0.42062737642585551</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="B33">
+        <f>MIN(C31,$C$2) - C31 * $C$2</f>
+        <v>0.21163517977706781</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>123</v>
+      </c>
+      <c r="B34" s="1">
+        <f>MIN($C$2, 0.5) - $C$2 * 0.5</f>
+        <v>0.23336501901140683</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>115</v>
+      </c>
+      <c r="B35">
+        <f>IF(C31 &lt;= 0.5, B33, B34)</f>
+        <v>0.23336501901140683</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>124</v>
+      </c>
+      <c r="B36" s="1">
+        <f>1/$C$2</f>
+        <v>1.8752228163992868</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="18">
+        <v>0</v>
+      </c>
+      <c r="B38" s="19"/>
+      <c r="C38" s="20"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" s="11">
+        <v>3796</v>
+      </c>
+      <c r="C39" s="22">
+        <f>B39/$B$1</f>
+        <v>0.45104562737642584</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="B40" s="11">
+        <v>2084</v>
+      </c>
+      <c r="C40" s="22">
+        <f>B40/$B$1</f>
+        <v>0.24762357414448669</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="B41" s="11">
+        <f>MIN(C39,$C$2) - C39 * $C$2</f>
+        <v>0.21051654281542306</v>
+      </c>
+      <c r="C41" s="22"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="B42" s="24">
+        <f>MIN($C$2, 0.5) - $C$2 * 0.5</f>
+        <v>0.23336501901140683</v>
+      </c>
+      <c r="C42" s="22"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="B43" s="11">
+        <f>IF(C39 &lt;= 0.5, B41, B42)</f>
+        <v>0.21051654281542306</v>
+      </c>
+      <c r="C43" s="22"/>
+    </row>
+    <row r="44" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="B44" s="26">
+        <f>1/$C$2</f>
+        <v>1.8752228163992868</v>
+      </c>
+      <c r="C44" s="27"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>125</v>
+      </c>
+      <c r="B47">
+        <v>3600</v>
+      </c>
+      <c r="C47" s="22">
+        <f>B47/$B$1</f>
+        <v>0.42775665399239543</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>126</v>
+      </c>
+      <c r="B48">
+        <v>1904</v>
+      </c>
+      <c r="C48" s="22">
+        <f>B48/$B$1</f>
+        <v>0.22623574144486691</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="B49" s="11">
+        <f>MIN(C47,$C$2) - C47 * $C$2</f>
+        <v>0.19964687938238226</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="B50" s="24">
+        <f>MIN($C$2, 0.5) - $C$2 * 0.5</f>
+        <v>0.23336501901140683</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="B51" s="11">
+        <f>IF(C47 &lt;= 0.5, B49, B50)</f>
+        <v>0.19964687938238226</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="B52" s="26">
+        <f>1/$C$2</f>
+        <v>1.8752228163992868</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="B53">
+        <f>C48 - C47 * $C$2</f>
+        <v>-1.874033165146255E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="B54">
+        <f>C48/(C47*$C$2)</f>
+        <v>0.99178451178451166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix bugs on calculating leverage
</commit_message>
<xml_diff>
--- a/File/Lattice.xlsx
+++ b/File/Lattice.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8880" yWindow="480" windowWidth="23060" windowHeight="14020" tabRatio="500" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="7780" yWindow="1320" windowWidth="23060" windowHeight="14020" tabRatio="500" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="FirstInIndex" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="5" r:id="rId4"/>
+    <sheet name="field19" sheetId="5" r:id="rId4"/>
+    <sheet name="field18&amp;field7" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="141">
   <si>
     <t>null</t>
   </si>
@@ -629,6 +630,30 @@
   </si>
   <si>
     <t>field19 = ONE/field6 = NONE/EDIBLE</t>
+  </si>
+  <si>
+    <t>field18 = WHITE</t>
+  </si>
+  <si>
+    <t>EDIBLE/field18 = WHITE</t>
+  </si>
+  <si>
+    <t>EDIBLE/field18 = WHITE/field6 = NONE</t>
+  </si>
+  <si>
+    <t>field18 = WHITE/field6 = NONE</t>
+  </si>
+  <si>
+    <t>field7 = FREE/field6 = NONE</t>
+  </si>
+  <si>
+    <t>EDIBLE/field7 = FREE/field6 = NONE</t>
+  </si>
+  <si>
+    <t>field19 = ONE/field9 = BROAD/field6 = NONE</t>
+  </si>
+  <si>
+    <t>EDIBLE/field19 = ONE/field9 = BROAD/field6 = NONE</t>
   </si>
 </sst>
 </file>
@@ -1729,8 +1754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2570,14 +2595,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14:F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -2747,7 +2772,7 @@
       </c>
       <c r="C16" s="12"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
         <v>98</v>
       </c>
@@ -2757,12 +2782,22 @@
       </c>
       <c r="C17" s="15"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E19" t="s">
+        <v>139</v>
+      </c>
+      <c r="F19">
+        <v>2944</v>
+      </c>
+      <c r="G19">
+        <f>F19/B1</f>
+        <v>0.34980988593155893</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>101</v>
       </c>
@@ -2773,8 +2808,18 @@
         <f>B20/$B$1</f>
         <v>0.6986692015209125</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E20" t="s">
+        <v>140</v>
+      </c>
+      <c r="F20">
+        <v>2944</v>
+      </c>
+      <c r="G20">
+        <f>F20/B1</f>
+        <v>0.34980988593155893</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
         <v>102</v>
       </c>
@@ -2784,6 +2829,278 @@
       <c r="C21" s="12">
         <f>B21/$B$1</f>
         <v>0.49619771863117873</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="10"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="12"/>
+      <c r="E22" t="s">
+        <v>129</v>
+      </c>
+      <c r="F22">
+        <f>G20-G19*C2</f>
+        <v>0.16326678136159262</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" s="11">
+        <f>C21/(C20*$C$2)</f>
+        <v>1.3317908981774529</v>
+      </c>
+      <c r="C23" s="12"/>
+      <c r="E23" t="s">
+        <v>130</v>
+      </c>
+      <c r="F23">
+        <f>G20/(G19*C2)</f>
+        <v>1.875222816399287</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" s="14">
+        <f>C21-C20*$C$2</f>
+        <v>0.1236184201014906</v>
+      </c>
+      <c r="C24" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="8">
+        <v>8416</v>
+      </c>
+      <c r="C1" s="9"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="11">
+        <v>4488</v>
+      </c>
+      <c r="C2" s="12">
+        <f>B2/$B$1</f>
+        <v>0.53326996197718635</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="14">
+        <v>3928</v>
+      </c>
+      <c r="C3" s="15">
+        <f>B3/$B$1</f>
+        <v>0.46673003802281371</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>129</v>
+      </c>
+      <c r="E5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6">
+        <v>8216</v>
+      </c>
+      <c r="C6" s="12">
+        <f>B6/$B$1</f>
+        <v>0.97623574144486691</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7">
+        <v>4296</v>
+      </c>
+      <c r="C7" s="12">
+        <f>B7/$B$1</f>
+        <v>0.51045627376425851</v>
+      </c>
+      <c r="D7">
+        <f>C7-C6*C2</f>
+        <v>-1.0140922956816012E-2</v>
+      </c>
+      <c r="E7">
+        <f>C7/(C6*C2)</f>
+        <v>0.98052059630615085</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8">
+        <v>3608</v>
+      </c>
+      <c r="C8" s="12">
+        <f>B8/$B$1</f>
+        <v>0.42870722433460073</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B9">
+        <v>3496</v>
+      </c>
+      <c r="C9" s="12">
+        <f>B9/$B$1</f>
+        <v>0.41539923954372626</v>
+      </c>
+      <c r="D9">
+        <f>C9-C2*C8</f>
+        <v>0.18678255432346863</v>
+      </c>
+      <c r="E9">
+        <f>C9/(C8*C2)</f>
+        <v>1.8170119085731451</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C10" s="11"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>129</v>
+      </c>
+      <c r="E11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B12">
+        <v>8200</v>
+      </c>
+      <c r="C12" s="12">
+        <f>B12/$B$1</f>
+        <v>0.9743346007604563</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13">
+        <v>4296</v>
+      </c>
+      <c r="C13" s="12">
+        <f>B13/$B$1</f>
+        <v>0.51045627376425851</v>
+      </c>
+      <c r="D13">
+        <f>C13-C12*C2</f>
+        <v>-9.1271017363270257E-3</v>
+      </c>
+      <c r="E13">
+        <f>C13/(C12*C2)</f>
+        <v>0.98243380722577267</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14">
+        <v>3616</v>
+      </c>
+      <c r="C14" s="12">
+        <f>B14/$B$1</f>
+        <v>0.42965779467680609</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>138</v>
+      </c>
+      <c r="B15">
+        <v>3496</v>
+      </c>
+      <c r="C15" s="12">
+        <f>B15/$B$1</f>
+        <v>0.41539923954372626</v>
+      </c>
+      <c r="D15">
+        <f>C15-C14*C2</f>
+        <v>0.18627564371322414</v>
+      </c>
+      <c r="E15">
+        <f>C15/(C14*C2)</f>
+        <v>1.8129919707223194</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" s="8">
+        <v>3808</v>
+      </c>
+      <c r="C20" s="9">
+        <f>B20/$B$1</f>
+        <v>0.45247148288973382</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="11">
+        <v>3688</v>
+      </c>
+      <c r="C21" s="12">
+        <f>B21/$B$1</f>
+        <v>0.43821292775665399</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -2792,23 +3109,13 @@
       <c r="C22" s="12"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="B23" s="11">
-        <f>C21/(C20*$C$2)</f>
-        <v>1.3317908981774529</v>
-      </c>
+      <c r="A23" s="10"/>
+      <c r="B23" s="11"/>
       <c r="C23" s="12"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="B24" s="14">
-        <f>C21-C20*$C$2</f>
-        <v>0.1236184201014906</v>
-      </c>
+      <c r="A24" s="13"/>
+      <c r="B24" s="14"/>
       <c r="C24" s="15"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix bugs for filtering itemsets
</commit_message>
<xml_diff>
--- a/File/Lattice.xlsx
+++ b/File/Lattice.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7780" yWindow="1320" windowWidth="23060" windowHeight="14020" tabRatio="500" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="9580" yWindow="780" windowWidth="23060" windowHeight="14020" tabRatio="500" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
     <sheet name="field19" sheetId="5" r:id="rId4"/>
     <sheet name="field18&amp;field7" sheetId="6" r:id="rId5"/>
+    <sheet name="field7&amp;field9&amp;field6" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="151">
   <si>
     <t>null</t>
   </si>
@@ -654,6 +655,36 @@
   </si>
   <si>
     <t>EDIBLE/field19 = ONE/field9 = BROAD/field6 = NONE</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S = 0.4153</t>
+  </si>
+  <si>
+    <t>{EDIBLE}</t>
+  </si>
+  <si>
+    <t>{field18 = WHITE, field6 = NONE}</t>
+  </si>
+  <si>
+    <t>S1 * S2</t>
+  </si>
+  <si>
+    <t>{field18 = WHITE}</t>
+  </si>
+  <si>
+    <t>{EDIBLE, field6 = NONE}</t>
+  </si>
+  <si>
+    <t>{field6 = NONE}</t>
+  </si>
+  <si>
+    <t>{EDIBLE, field18 = WHITE}</t>
   </si>
 </sst>
 </file>
@@ -2596,7 +2627,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="A12" sqref="A12:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2877,7 +2908,301 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="8">
+        <v>8416</v>
+      </c>
+      <c r="C1" s="9"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="11">
+        <v>4488</v>
+      </c>
+      <c r="C2" s="12">
+        <f>B2/$B$1</f>
+        <v>0.53326996197718635</v>
+      </c>
+      <c r="I2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="14">
+        <v>3928</v>
+      </c>
+      <c r="C3" s="15">
+        <f>B3/$B$1</f>
+        <v>0.46673003802281371</v>
+      </c>
+      <c r="G3" t="s">
+        <v>141</v>
+      </c>
+      <c r="H3" t="s">
+        <v>142</v>
+      </c>
+      <c r="I3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>144</v>
+      </c>
+      <c r="H4" t="s">
+        <v>145</v>
+      </c>
+      <c r="I4">
+        <f>C2*C8</f>
+        <v>0.22861668522025763</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>129</v>
+      </c>
+      <c r="E5" t="s">
+        <v>130</v>
+      </c>
+      <c r="G5" t="s">
+        <v>147</v>
+      </c>
+      <c r="H5" t="s">
+        <v>148</v>
+      </c>
+      <c r="I5">
+        <f>C6*C21</f>
+        <v>0.42779912243924301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6">
+        <v>8216</v>
+      </c>
+      <c r="C6" s="12">
+        <f>B6/$B$1</f>
+        <v>0.97623574144486691</v>
+      </c>
+      <c r="G6" t="s">
+        <v>149</v>
+      </c>
+      <c r="H6" t="s">
+        <v>150</v>
+      </c>
+      <c r="I6">
+        <f>C20*C7</f>
+        <v>0.23096690714048199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7">
+        <v>4296</v>
+      </c>
+      <c r="C7" s="12">
+        <f>B7/$B$1</f>
+        <v>0.51045627376425851</v>
+      </c>
+      <c r="D7">
+        <f>C7-C6*C2</f>
+        <v>-1.0140922956816012E-2</v>
+      </c>
+      <c r="E7">
+        <f>C7/(C6*C2)</f>
+        <v>0.98052059630615085</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8">
+        <v>3608</v>
+      </c>
+      <c r="C8" s="12">
+        <f>B8/$B$1</f>
+        <v>0.42870722433460073</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B9">
+        <v>3496</v>
+      </c>
+      <c r="C9" s="12">
+        <f>B9/$B$1</f>
+        <v>0.41539923954372626</v>
+      </c>
+      <c r="D9">
+        <f>C9-C2*C8</f>
+        <v>0.18678255432346863</v>
+      </c>
+      <c r="E9">
+        <f>C9/(C8*C2)</f>
+        <v>1.8170119085731451</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C10" s="11"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>129</v>
+      </c>
+      <c r="E11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B12">
+        <v>8200</v>
+      </c>
+      <c r="C12" s="12">
+        <f>B12/$B$1</f>
+        <v>0.9743346007604563</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13">
+        <v>4296</v>
+      </c>
+      <c r="C13" s="12">
+        <f>B13/$B$1</f>
+        <v>0.51045627376425851</v>
+      </c>
+      <c r="D13">
+        <f>C13-C12*C2</f>
+        <v>-9.1271017363270257E-3</v>
+      </c>
+      <c r="E13">
+        <f>C13/(C12*C2)</f>
+        <v>0.98243380722577267</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14">
+        <v>3616</v>
+      </c>
+      <c r="C14" s="12">
+        <f>B14/$B$1</f>
+        <v>0.42965779467680609</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>138</v>
+      </c>
+      <c r="B15">
+        <v>3496</v>
+      </c>
+      <c r="C15" s="12">
+        <f>B15/$B$1</f>
+        <v>0.41539923954372626</v>
+      </c>
+      <c r="D15">
+        <f>C15-C14*C2</f>
+        <v>0.18627564371322414</v>
+      </c>
+      <c r="E15">
+        <f>C15/(C14*C2)</f>
+        <v>1.8129919707223194</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" s="8">
+        <v>3808</v>
+      </c>
+      <c r="C20" s="9">
+        <f>B20/$B$1</f>
+        <v>0.45247148288973382</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="11">
+        <v>3688</v>
+      </c>
+      <c r="C21" s="12">
+        <f>B21/$B$1</f>
+        <v>0.43821292775665399</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="10"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="12"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="10"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="12"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="13"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
@@ -2885,10 +3210,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>87</v>
       </c>
@@ -2897,7 +3222,7 @@
       </c>
       <c r="C1" s="9"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>88</v>
       </c>
@@ -2909,7 +3234,7 @@
         <v>0.53326996197718635</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>89</v>
       </c>
@@ -2921,202 +3246,188 @@
         <v>0.46673003802281371</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>129</v>
-      </c>
-      <c r="E5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>133</v>
-      </c>
-      <c r="B6">
-        <v>8216</v>
-      </c>
-      <c r="C6" s="12">
-        <f>B6/$B$1</f>
-        <v>0.97623574144486691</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>134</v>
-      </c>
-      <c r="B7">
-        <v>4296</v>
-      </c>
-      <c r="C7" s="12">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="8">
+        <v>3808</v>
+      </c>
+      <c r="C7" s="9">
         <f>B7/$B$1</f>
-        <v>0.51045627376425851</v>
-      </c>
-      <c r="D7">
-        <f>C7-C6*C2</f>
-        <v>-1.0140922956816012E-2</v>
-      </c>
-      <c r="E7">
-        <f>C7/(C6*C2)</f>
-        <v>0.98052059630615085</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>136</v>
-      </c>
-      <c r="B8">
-        <v>3608</v>
+        <v>0.45247148288973382</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="11">
+        <v>3688</v>
       </c>
       <c r="C8" s="12">
         <f>B8/$B$1</f>
-        <v>0.42870722433460073</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>135</v>
-      </c>
-      <c r="B9">
-        <v>3496</v>
-      </c>
-      <c r="C9" s="12">
-        <f>B9/$B$1</f>
-        <v>0.41539923954372626</v>
-      </c>
-      <c r="D9">
-        <f>C9-C2*C8</f>
-        <v>0.18678255432346863</v>
-      </c>
-      <c r="E9">
-        <f>C9/(C8*C2)</f>
-        <v>1.8170119085731451</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C10" s="11"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
-        <v>129</v>
-      </c>
-      <c r="E11" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>113</v>
-      </c>
-      <c r="B12">
-        <v>8200</v>
-      </c>
-      <c r="C12" s="12">
-        <f>B12/$B$1</f>
-        <v>0.9743346007604563</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>114</v>
-      </c>
-      <c r="B13">
-        <v>4296</v>
-      </c>
-      <c r="C13" s="12">
-        <f>B13/$B$1</f>
-        <v>0.51045627376425851</v>
-      </c>
-      <c r="D13">
-        <f>C13-C12*C2</f>
-        <v>-9.1271017363270257E-3</v>
-      </c>
-      <c r="E13">
-        <f>C13/(C12*C2)</f>
-        <v>0.98243380722577267</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>137</v>
-      </c>
-      <c r="B14">
-        <v>3616</v>
-      </c>
-      <c r="C14" s="12">
+        <v>0.43821292775665399</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" s="11">
+        <f>C8/(C7*$C$2)</f>
+        <v>1.8161296604203176</v>
+      </c>
+      <c r="C10" s="12"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" s="14">
+        <f>C8-C7*$C$2</f>
+        <v>0.1969234772802845</v>
+      </c>
+      <c r="C11" s="15"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B14" s="8">
+        <v>5880</v>
+      </c>
+      <c r="C14" s="9">
         <f>B14/$B$1</f>
-        <v>0.42965779467680609</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>138</v>
-      </c>
-      <c r="B15">
-        <v>3496</v>
+        <v>0.6986692015209125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15" s="11">
+        <v>4176</v>
       </c>
       <c r="C15" s="12">
         <f>B15/$B$1</f>
+        <v>0.49619771863117873</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="10"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="12"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="11">
+        <f>C15/(C14*$C$2)</f>
+        <v>1.3317908981774529</v>
+      </c>
+      <c r="C17" s="12"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B18" s="14">
+        <f>C15-C14*$C$2</f>
+        <v>0.1236184201014906</v>
+      </c>
+      <c r="C18" s="15"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>129</v>
+      </c>
+      <c r="E21" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22">
+        <v>8200</v>
+      </c>
+      <c r="C22" s="12">
+        <f>B22/$B$1</f>
+        <v>0.9743346007604563</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23">
+        <v>4296</v>
+      </c>
+      <c r="C23" s="12">
+        <f>B23/$B$1</f>
+        <v>0.51045627376425851</v>
+      </c>
+      <c r="D23">
+        <f>C23-C22*C2</f>
+        <v>-9.1271017363270257E-3</v>
+      </c>
+      <c r="E23">
+        <f>C23/(C22*C2)</f>
+        <v>0.98243380722577267</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>137</v>
+      </c>
+      <c r="B24">
+        <v>3616</v>
+      </c>
+      <c r="C24" s="12">
+        <f>B24/$B$1</f>
+        <v>0.42965779467680609</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>138</v>
+      </c>
+      <c r="B25">
+        <v>3496</v>
+      </c>
+      <c r="C25" s="12">
+        <f>B25/$B$1</f>
         <v>0.41539923954372626</v>
       </c>
-      <c r="D15">
-        <f>C15-C14*C2</f>
+      <c r="D25">
+        <f>C25-C24*C2</f>
         <v>0.18627564371322414</v>
       </c>
-      <c r="E15">
-        <f>C15/(C14*C2)</f>
+      <c r="E25">
+        <f>C25/(C24*C2)</f>
         <v>1.8129919707223194</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B20" s="8">
-        <v>3808</v>
-      </c>
-      <c r="C20" s="9">
-        <f>B20/$B$1</f>
-        <v>0.45247148288973382</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="B21" s="11">
-        <v>3688</v>
-      </c>
-      <c r="C21" s="12">
-        <f>B21/$B$1</f>
-        <v>0.43821292775665399</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="10"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="12"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="10"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="12"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="13"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update with prove of self-sufficient itemset
</commit_message>
<xml_diff>
--- a/File/Lattice.xlsx
+++ b/File/Lattice.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="800" yWindow="8680" windowWidth="23060" windowHeight="14020" tabRatio="500" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="1140" yWindow="1400" windowWidth="29920" windowHeight="14020" tabRatio="500" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="FirstInIndex" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
     <sheet name="field19" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="10" r:id="rId5"/>
+    <sheet name="p-value" sheetId="10" r:id="rId5"/>
     <sheet name="field18&amp;field7" sheetId="6" r:id="rId6"/>
     <sheet name="field7&amp;field9&amp;field6" sheetId="7" r:id="rId7"/>
     <sheet name="Lift" sheetId="8" r:id="rId8"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="181">
   <si>
     <t>null</t>
   </si>
@@ -551,24 +551,12 @@
     <t>field6 = NONE/field9 = BROAD</t>
   </si>
   <si>
-    <t>checkSubsets(item = -1, is = [-1, 49,31], cnt = 3472, new_sup = 0.412547528, parentCnt = 3544, parentSup = 0.42110267, alpha = 0.05)</t>
-  </si>
-  <si>
     <t>49, 31, -1</t>
   </si>
   <si>
     <t>EDIBLE/field6 = NONE/field9 = BROAD</t>
   </si>
   <si>
-    <t>sofar = [-1]</t>
-  </si>
-  <si>
-    <t>remaining = [49, 31]</t>
-  </si>
-  <si>
-    <t>checkSubsetsX(sofar = [49, -1], remaining = [31], limit = 49, cnt = 3472, new_sup = 0.412547, alpha = 0.05)</t>
-  </si>
-  <si>
     <t>-1, 49, 31, 18</t>
   </si>
   <si>
@@ -749,13 +737,49 @@
     <t>ad, bc</t>
   </si>
   <si>
-    <t>P</t>
-  </si>
-  <si>
     <t>BigML(7.0858E-58)</t>
   </si>
   <si>
     <t>FISHER addIn</t>
+  </si>
+  <si>
+    <t>OpusMiner</t>
+  </si>
+  <si>
+    <t>1.00000000009649</t>
+  </si>
+  <si>
+    <t>BigML(4.28846E-26)</t>
+  </si>
+  <si>
+    <t>a, cd</t>
+  </si>
+  <si>
+    <t>c, ad</t>
+  </si>
+  <si>
+    <t>d, ac</t>
+  </si>
+  <si>
+    <t>Exclusive domain of field19 = ONE is 648</t>
+  </si>
+  <si>
+    <t>support</t>
+  </si>
+  <si>
+    <t>EDIBLE/field6 = NONE/field9 = BROAD/ edom(S)</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>cov(S1) &amp; edom(S)</t>
+  </si>
+  <si>
+    <t>cov(S2) &amp; edom(S)</t>
+  </si>
+  <si>
+    <t>RHS</t>
   </si>
 </sst>
 </file>
@@ -810,7 +834,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -832,6 +856,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1023,7 +1053,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1056,6 +1086,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1068,6 +1102,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>147578</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4051300" y="177800"/>
+          <a:ext cx="5702300" cy="579378"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1873,13 +1956,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:C16"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2078,12 +2162,12 @@
       </c>
       <c r="C16" s="15"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>101</v>
       </c>
@@ -2095,7 +2179,7 @@
         <v>0.6986692015209125</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
         <v>102</v>
       </c>
@@ -2107,15 +2191,12 @@
         <v>0.49619771863117873</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="10"/>
       <c r="B21" s="11"/>
       <c r="C21" s="12"/>
-      <c r="E21" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
         <v>97</v>
       </c>
@@ -2125,7 +2206,7 @@
       </c>
       <c r="C22" s="12"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
         <v>98</v>
       </c>
@@ -2135,22 +2216,14 @@
       </c>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E24" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="9"/>
-      <c r="E25" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">
         <v>103</v>
       </c>
@@ -2161,13 +2234,10 @@
         <f>B26/$B$1</f>
         <v>0.42110266159695819</v>
       </c>
-      <c r="E26" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B27" s="11">
         <v>3472</v>
@@ -2177,7 +2247,7 @@
         <v>0.41254752851711024</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
         <v>97</v>
       </c>
@@ -2187,7 +2257,7 @@
       </c>
       <c r="C28" s="12"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="13" t="s">
         <v>98</v>
       </c>
@@ -2197,14 +2267,14 @@
       </c>
       <c r="C29" s="15"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B32">
         <v>2328</v>
@@ -2216,7 +2286,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B33">
         <v>2256</v>
@@ -2302,7 +2372,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B6">
         <v>8200</v>
@@ -2314,7 +2384,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B7">
         <v>4296</v>
@@ -2326,7 +2396,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B8">
         <f>MIN(C6,$C$2) - C6 * $C$2</f>
@@ -2335,7 +2405,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B9" s="1">
         <f>MIN($C$2, 0.5) - $C$2 * 0.5</f>
@@ -2344,7 +2414,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B10">
         <f>IF(C6 &lt;= 0.5, B8, B9)</f>
@@ -2353,7 +2423,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B11" s="1">
         <f>1/$C$2</f>
@@ -2367,7 +2437,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B14">
         <v>4864</v>
@@ -2379,7 +2449,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B15">
         <v>2848</v>
@@ -2391,7 +2461,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B16">
         <f>MIN(C14,$C$2) - C14 * $C$2</f>
@@ -2400,7 +2470,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B17" s="1">
         <f>MIN($C$2, 0.5) - $C$2 * 0.5</f>
@@ -2409,7 +2479,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B18">
         <f>IF(C14 &lt;= 0.5, B16, B17)</f>
@@ -2418,7 +2488,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B19" s="1">
         <f>1/$C$2</f>
@@ -2432,7 +2502,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B23">
         <v>5316</v>
@@ -2444,7 +2514,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B24">
         <v>3780</v>
@@ -2456,7 +2526,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B25">
         <f>MIN(C23,$C$2) - C23 * $C$2</f>
@@ -2465,7 +2535,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B26" s="1">
         <f>MIN($C$2, 0.5) - $C$2 * 0.5</f>
@@ -2474,7 +2544,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B27">
         <f>IF(C23 &lt;= 0.5, B25, B26)</f>
@@ -2483,7 +2553,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B28" s="1">
         <f>1/$C$2</f>
@@ -2497,7 +2567,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B31">
         <v>5076</v>
@@ -2509,7 +2579,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B32">
         <v>3540</v>
@@ -2521,7 +2591,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B33">
         <f>MIN(C31,$C$2) - C31 * $C$2</f>
@@ -2530,7 +2600,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B34" s="1">
         <f>MIN($C$2, 0.5) - $C$2 * 0.5</f>
@@ -2539,7 +2609,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B35">
         <f>IF(C31 &lt;= 0.5, B33, B34)</f>
@@ -2548,7 +2618,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B36" s="1">
         <f>1/$C$2</f>
@@ -2589,7 +2659,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="23" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B41" s="11">
         <f>MIN(C39,$C$2) - C39 * $C$2</f>
@@ -2599,7 +2669,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="21" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B42" s="24">
         <f>MIN($C$2, 0.5) - $C$2 * 0.5</f>
@@ -2609,7 +2679,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="21" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B43" s="11">
         <f>IF(C39 &lt;= 0.5, B41, B42)</f>
@@ -2619,7 +2689,7 @@
     </row>
     <row r="44" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="25" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B44" s="26">
         <f>1/$C$2</f>
@@ -2629,7 +2699,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B47">
         <v>3600</v>
@@ -2641,7 +2711,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B48">
         <v>1904</v>
@@ -2653,7 +2723,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="23" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B49" s="11">
         <f>MIN(C47,$C$2) - C47 * $C$2</f>
@@ -2662,7 +2732,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="21" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B50" s="24">
         <f>MIN($C$2, 0.5) - $C$2 * 0.5</f>
@@ -2671,7 +2741,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="21" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B51" s="11">
         <f>IF(C47 &lt;= 0.5, B49, B50)</f>
@@ -2680,7 +2750,7 @@
     </row>
     <row r="52" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="25" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B52" s="26">
         <f>1/$C$2</f>
@@ -2689,7 +2759,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="28" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B53">
         <f>C48 - C47 * $C$2</f>
@@ -2698,7 +2768,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="28" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B54">
         <f>C48/(C47*$C$2)</f>
@@ -2712,19 +2782,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.83203125" customWidth="1"/>
+    <col min="11" max="11" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>87</v>
       </c>
@@ -2733,7 +2806,7 @@
       </c>
       <c r="C1" s="9"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>88</v>
       </c>
@@ -2745,7 +2818,7 @@
         <v>0.53326996197718635</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>89</v>
       </c>
@@ -2756,15 +2829,21 @@
         <f>B3/$B$1</f>
         <v>0.46673003802281371</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J3" t="s">
+        <v>174</v>
+      </c>
+      <c r="L3">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B6" s="8">
         <v>7768</v>
@@ -2774,12 +2853,24 @@
         <v>0.9230038022813688</v>
       </c>
       <c r="E6" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+      <c r="L6" t="s">
+        <v>175</v>
+      </c>
+      <c r="M6" t="s">
+        <v>178</v>
+      </c>
+      <c r="N6" t="s">
+        <v>179</v>
+      </c>
+      <c r="O6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B7" s="11">
         <v>3960</v>
@@ -2788,25 +2879,85 @@
         <f>B7/$B$1</f>
         <v>0.47053231939163498</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J7" t="s">
+        <v>88</v>
+      </c>
+      <c r="K7" t="s">
+        <v>103</v>
+      </c>
+      <c r="L7">
+        <f>C2*C27</f>
+        <v>0.22456140033830185</v>
+      </c>
+      <c r="M7">
+        <v>528</v>
+      </c>
+      <c r="N7">
+        <v>600</v>
+      </c>
+      <c r="O7">
+        <f>(M7*N7)/$L$3</f>
+        <v>488.88888888888891</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J8" t="s">
+        <v>99</v>
+      </c>
+      <c r="K8" t="s">
+        <v>102</v>
+      </c>
+      <c r="L8">
+        <f>C13*C21</f>
+        <v>0.22451531755555235</v>
+      </c>
+      <c r="M8">
+        <v>600</v>
+      </c>
+      <c r="N8">
+        <v>528</v>
+      </c>
+      <c r="O8">
+        <f t="shared" ref="O8:O9" si="0">(M8*N8)/$L$3</f>
+        <v>488.88888888888891</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B9" s="11">
         <f>C7-C6*C2</f>
         <v>-2.1677883155748978E-2</v>
       </c>
       <c r="C9" s="12"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J9" t="s">
+        <v>101</v>
+      </c>
+      <c r="K9" t="s">
+        <v>100</v>
+      </c>
+      <c r="L9">
+        <f>C20*C14</f>
+        <v>0.30616587633188275</v>
+      </c>
+      <c r="M9">
+        <v>648</v>
+      </c>
+      <c r="N9">
+        <v>528</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>528</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B10" s="14">
         <f>C7/(C6*C2)</f>
@@ -2814,9 +2965,9 @@
       </c>
       <c r="C10" s="15"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E11" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F11">
         <v>3208</v>
@@ -2825,13 +2976,22 @@
         <f>F11/$B$1</f>
         <v>0.38117870722433461</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I11" t="s">
+        <v>177</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="K11">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F12">
         <v>3160</v>
@@ -2841,7 +3001,7 @@
         <v>0.37547528517110268</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>99</v>
       </c>
@@ -2853,7 +3013,7 @@
         <v>0.45247148288973382</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
         <v>100</v>
       </c>
@@ -2865,26 +3025,26 @@
         <v>0.43821292775665399</v>
       </c>
       <c r="E14" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F14">
         <f>G12-G11*C2</f>
         <v>0.17220413046306871</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="12"/>
       <c r="E15" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F15">
         <f>G12/(G11*C2)</f>
         <v>1.8471646196451827</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
         <v>97</v>
       </c>
@@ -2909,7 +3069,7 @@
         <v>31</v>
       </c>
       <c r="E19" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F19">
         <v>2944</v>
@@ -2931,7 +3091,7 @@
         <v>0.6986692015209125</v>
       </c>
       <c r="E20" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F20">
         <v>2944</v>
@@ -2958,7 +3118,7 @@
       <c r="B22" s="11"/>
       <c r="C22" s="12"/>
       <c r="E22" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F22">
         <f>G20-G19*C2</f>
@@ -2975,7 +3135,7 @@
       </c>
       <c r="C23" s="12"/>
       <c r="E23" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F23">
         <f>G20/(G19*C2)</f>
@@ -2992,9 +3152,31 @@
       </c>
       <c r="C24" s="15"/>
     </row>
+    <row r="27" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A27" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" s="11">
+        <v>3544</v>
+      </c>
+      <c r="C27">
+        <f>B27/B1</f>
+        <v>0.42110266159695819</v>
+      </c>
+    </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" s="11">
+        <v>3472</v>
+      </c>
+      <c r="C28">
+        <f>B28/B1</f>
+        <v>0.41254752851711024</v>
+      </c>
       <c r="E28" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F28">
         <v>1112</v>
@@ -3006,7 +3188,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E29" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F29">
         <v>1000</v>
@@ -3024,7 +3206,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E32" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F32">
         <v>1232</v>
@@ -3036,7 +3218,7 @@
     </row>
     <row r="33" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E33" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F33">
         <v>980</v>
@@ -3054,24 +3236,27 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -3110,7 +3295,7 @@
         <v>88</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>101</v>
@@ -3142,13 +3327,13 @@
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F5" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -3156,7 +3341,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C6">
         <v>4488</v>
@@ -3167,7 +3352,7 @@
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>0</v>
       </c>
       <c r="J6" t="s">
@@ -3182,7 +3367,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C7" s="8">
         <v>7768</v>
@@ -3190,22 +3375,22 @@
       <c r="D7">
         <v>3472</v>
       </c>
-      <c r="E7" s="29">
-        <v>2.9099999999999999E-106</v>
-      </c>
-      <c r="F7" s="29">
+      <c r="E7" s="30">
         <v>7.5999999999999999E-106</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>169</v>
       </c>
       <c r="I7" t="s">
         <v>93</v>
       </c>
       <c r="J7">
         <f>L9-K9-L8+K8</f>
-        <v>3928</v>
+        <v>2440</v>
       </c>
       <c r="K7">
         <f>K9-K8</f>
-        <v>1544</v>
+        <v>744</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -3213,7 +3398,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C8" s="8">
         <v>5880</v>
@@ -3224,7 +3409,7 @@
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>0</v>
       </c>
       <c r="I8" t="s">
@@ -3232,13 +3417,13 @@
       </c>
       <c r="J8">
         <f>L8-K8</f>
-        <v>0</v>
+        <v>2288</v>
       </c>
       <c r="K8">
         <v>2944</v>
       </c>
       <c r="L8">
-        <v>2944</v>
+        <v>5232</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -3246,7 +3431,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C9" s="8">
         <v>3808</v>
@@ -3257,11 +3442,11 @@
       <c r="E9">
         <v>0</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>0</v>
       </c>
       <c r="K9">
-        <v>4488</v>
+        <v>3688</v>
       </c>
       <c r="L9">
         <v>8416</v>
@@ -3272,7 +3457,7 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C10" s="11">
         <v>3960</v>
@@ -3283,11 +3468,7 @@
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <f>[1]!fet(J7,K7,J8,K8)</f>
+      <c r="G10">
         <v>0</v>
       </c>
     </row>
@@ -3296,19 +3477,19 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C11" s="8">
-        <v>5880</v>
+        <v>4176</v>
       </c>
       <c r="D11">
         <v>3208</v>
       </c>
-      <c r="E11" s="29">
-        <v>1.5076999999999999E-293</v>
-      </c>
-      <c r="F11" s="29">
-        <v>1.5076999999999999E-293</v>
+      <c r="E11" s="32">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -3316,7 +3497,7 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C12" s="11">
         <v>3688</v>
@@ -3324,11 +3505,176 @@
       <c r="D12">
         <v>5232</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="33">
+        <v>6.6020999999999996E-199</v>
+      </c>
+      <c r="G12" s="29">
+        <v>6.6020823731771101E-199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>-1</v>
+      </c>
+      <c r="B18">
+        <v>31</v>
+      </c>
+      <c r="C18">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>4488</v>
+      </c>
+      <c r="B20" s="8">
+        <v>5880</v>
+      </c>
+      <c r="C20" s="8">
+        <v>3808</v>
+      </c>
+      <c r="D20" s="28">
+        <v>3472</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
+        <v>167</v>
+      </c>
+      <c r="F21" t="s">
+        <v>170</v>
+      </c>
+      <c r="G21" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>171</v>
+      </c>
+      <c r="C22">
+        <v>4488</v>
+      </c>
+      <c r="D22">
+        <v>3544</v>
+      </c>
+      <c r="E22">
         <v>0</v>
       </c>
-      <c r="F12" s="29">
-        <v>6.6020999999999996E-199</v>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="J22" t="s">
+        <v>90</v>
+      </c>
+      <c r="K22" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>172</v>
+      </c>
+      <c r="C23">
+        <v>5880</v>
+      </c>
+      <c r="D23">
+        <v>3960</v>
+      </c>
+      <c r="E23" s="29">
+        <v>5.4391872495198214E-262</v>
+      </c>
+      <c r="G23" s="29">
+        <v>5.4391872495483502E-262</v>
+      </c>
+      <c r="I23" t="s">
+        <v>93</v>
+      </c>
+      <c r="J23">
+        <f>L25-K25-L24+K24</f>
+        <v>3904</v>
+      </c>
+      <c r="K23">
+        <f>K25-K24</f>
+        <v>704</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>173</v>
+      </c>
+      <c r="C24">
+        <v>3808</v>
+      </c>
+      <c r="D24">
+        <v>4176</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="I24" t="s">
+        <v>95</v>
+      </c>
+      <c r="J24">
+        <f>L24-K24</f>
+        <v>336</v>
+      </c>
+      <c r="K24">
+        <v>3472</v>
+      </c>
+      <c r="L24">
+        <v>3808</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K25">
+        <v>4176</v>
+      </c>
+      <c r="L25">
+        <v>8416</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I27">
+        <f>[1]!fet(J23,K23,J24,K24)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3372,7 +3718,7 @@
         <v>0.53326996197718635</v>
       </c>
       <c r="I2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -3387,21 +3733,21 @@
         <v>0.46673003802281371</v>
       </c>
       <c r="G3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="H3" t="s">
+        <v>138</v>
+      </c>
+      <c r="I3" t="s">
         <v>142</v>
-      </c>
-      <c r="I3" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="H4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="I4">
         <f>C2*C8</f>
@@ -3413,16 +3759,16 @@
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H5" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="I5">
         <f>C6*C21</f>
@@ -3431,7 +3777,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B6">
         <v>8216</v>
@@ -3441,10 +3787,10 @@
         <v>0.97623574144486691</v>
       </c>
       <c r="G6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H6" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="I6">
         <f>C20*C7</f>
@@ -3453,7 +3799,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B7">
         <v>4296</v>
@@ -3473,7 +3819,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B8">
         <v>3608</v>
@@ -3485,7 +3831,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B9">
         <v>3496</v>
@@ -3511,15 +3857,15 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E11" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B12">
         <v>8200</v>
@@ -3531,7 +3877,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B13">
         <v>4296</v>
@@ -3551,7 +3897,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B14">
         <v>3616</v>
@@ -3563,7 +3909,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B15">
         <v>3496</v>
@@ -3789,15 +4135,15 @@
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E21" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B22">
         <v>8200</v>
@@ -3809,7 +4155,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B23">
         <v>4296</v>
@@ -3829,7 +4175,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B24">
         <v>3616</v>
@@ -3841,7 +4187,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B25">
         <v>3496</v>
@@ -3921,7 +4267,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B7">
         <v>2096</v>
@@ -3933,7 +4279,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B8">
         <v>1872</v>
@@ -3950,7 +4296,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B14">
         <v>216</v>
@@ -3962,7 +4308,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B15">
         <v>192</v>
@@ -3974,12 +4320,12 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D17" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B18">
         <v>48</v>
@@ -3995,7 +4341,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B23">
         <v>16</v>
@@ -4003,7 +4349,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B24">
         <v>16</v>

</xml_diff>

<commit_message>
Update questions and new testing result
</commit_message>
<xml_diff>
--- a/File/Lattice.xlsx
+++ b/File/Lattice.xlsx
@@ -9,20 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1400" windowWidth="29920" windowHeight="14020" tabRatio="500" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="3280" yWindow="920" windowWidth="19760" windowHeight="14020" tabRatio="500" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="FirstInIndex" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
     <sheet name="field19" sheetId="5" r:id="rId4"/>
-    <sheet name="p-value" sheetId="10" r:id="rId5"/>
-    <sheet name="field18&amp;field7" sheetId="6" r:id="rId6"/>
-    <sheet name="field7&amp;field9&amp;field6" sheetId="7" r:id="rId7"/>
-    <sheet name="Lift" sheetId="8" r:id="rId8"/>
+    <sheet name="Adult" sheetId="11" r:id="rId5"/>
+    <sheet name="p-value" sheetId="10" r:id="rId6"/>
+    <sheet name="field18&amp;field7" sheetId="6" r:id="rId7"/>
+    <sheet name="field7&amp;field9&amp;field6" sheetId="7" r:id="rId8"/>
+    <sheet name="Lift" sheetId="8" r:id="rId9"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId9"/>
+    <externalReference r:id="rId10"/>
   </externalReferences>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="202">
   <si>
     <t>null</t>
   </si>
@@ -780,6 +781,69 @@
   </si>
   <si>
     <t>RHS</t>
+  </si>
+  <si>
+    <t>&gt;50K</t>
+  </si>
+  <si>
+    <t>&lt;=50K</t>
+  </si>
+  <si>
+    <t>field1 = Age41-50</t>
+  </si>
+  <si>
+    <t>field4 = EduNum15</t>
+  </si>
+  <si>
+    <t>field2 = Self-emp-inc</t>
+  </si>
+  <si>
+    <t>&gt;50K &amp; field1 = Age41-50 &amp; field4 = EduNum15 &amp; field2 = Self-emp-inc</t>
+  </si>
+  <si>
+    <t>field1 = Age41-50 &amp; field4 = EduNum15 &amp; field2 = Self-emp-inc</t>
+  </si>
+  <si>
+    <t>field6 = Exec-managerial (Exclusive domain)</t>
+  </si>
+  <si>
+    <t>&gt;50K &amp; field1 = Age41-50 &amp; field4 = EduNum15 &amp; field2 = Self-emp-inc &amp; edom()</t>
+  </si>
+  <si>
+    <t>&gt;50K &amp; field4 = EduNum15 &amp; field2 = Self-emp-inc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">field1 = Age41-50 </t>
+  </si>
+  <si>
+    <t>&gt;50K &amp; field1 = Age41-50 &amp; field2 = Self-emp-inc</t>
+  </si>
+  <si>
+    <t>&gt;50K &amp; field1 = Age41-50 &amp; field4 = EduNum15</t>
+  </si>
+  <si>
+    <t>&gt;50K &amp; field1 = Age41-50</t>
+  </si>
+  <si>
+    <t>field4 = EduNum15 &amp; field2 = Self-emp-inc</t>
+  </si>
+  <si>
+    <t>field1 = Age41-50 &amp; field2 = Self-emp-inc</t>
+  </si>
+  <si>
+    <t>&gt;50K &amp; field4 = EduNum15</t>
+  </si>
+  <si>
+    <t>field1 = Age41-50 &amp; field4 = EduNum15</t>
+  </si>
+  <si>
+    <t>&gt;50K &amp; field2 = Self-emp-inc</t>
+  </si>
+  <si>
+    <t>Itemset</t>
+  </si>
+  <si>
+    <t>field10 = Hour36-50 (Exclusive domain)</t>
   </si>
 </sst>
 </file>
@@ -1153,6 +1217,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2616200</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>134878</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4419600" y="165100"/>
+          <a:ext cx="5702300" cy="579378"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -2784,8 +2897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6:O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3241,6 +3354,426 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="7.83203125" customWidth="1"/>
+    <col min="7" max="7" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="52.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="8">
+        <v>32561</v>
+      </c>
+      <c r="C1" s="9"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="B2" s="11">
+        <v>7841</v>
+      </c>
+      <c r="C2" s="12">
+        <f>B2/$B$1</f>
+        <v>0.24080955744602439</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B3" s="14">
+        <f>B1-B2</f>
+        <v>24720</v>
+      </c>
+      <c r="C3" s="15">
+        <f>B3/$B$1</f>
+        <v>0.75919044255397561</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B6">
+        <v>6983</v>
+      </c>
+      <c r="C6">
+        <f>B6/$B$1</f>
+        <v>0.21445901538650533</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B8">
+        <v>576</v>
+      </c>
+      <c r="C8">
+        <f>B8/$B$1</f>
+        <v>1.7689874389607198E-2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>188</v>
+      </c>
+      <c r="H8">
+        <v>28495</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>185</v>
+      </c>
+      <c r="B10">
+        <v>1116</v>
+      </c>
+      <c r="C10">
+        <f>B10/$B$1</f>
+        <v>3.4274131629863945E-2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>137</v>
+      </c>
+      <c r="H10" t="s">
+        <v>138</v>
+      </c>
+      <c r="I10" t="s">
+        <v>178</v>
+      </c>
+      <c r="J10" t="s">
+        <v>179</v>
+      </c>
+      <c r="K10" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G11" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="H11" t="s">
+        <v>187</v>
+      </c>
+      <c r="I11">
+        <v>5873</v>
+      </c>
+      <c r="J11">
+        <v>34</v>
+      </c>
+      <c r="K11">
+        <f>(I11*J11)/$H$8</f>
+        <v>7.0076153711177396</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>191</v>
+      </c>
+      <c r="H12" t="s">
+        <v>190</v>
+      </c>
+      <c r="I12">
+        <v>5794</v>
+      </c>
+      <c r="J12">
+        <v>74</v>
+      </c>
+      <c r="K12">
+        <f>(I12*J12)/$H$8</f>
+        <v>15.046709949113879</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>184</v>
+      </c>
+      <c r="H13" t="s">
+        <v>192</v>
+      </c>
+      <c r="I13">
+        <v>524</v>
+      </c>
+      <c r="J13">
+        <v>135</v>
+      </c>
+      <c r="K13">
+        <f>(I13*J13)/$H$8</f>
+        <v>2.482540796630988</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>200</v>
+      </c>
+      <c r="G14" t="s">
+        <v>185</v>
+      </c>
+      <c r="H14" t="s">
+        <v>193</v>
+      </c>
+      <c r="I14">
+        <v>716</v>
+      </c>
+      <c r="J14">
+        <v>150</v>
+      </c>
+      <c r="K14">
+        <f>(I14*J14)/$H$8</f>
+        <v>3.7690822951394982</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>186</v>
+      </c>
+      <c r="G15" t="s">
+        <v>194</v>
+      </c>
+      <c r="H15" t="s">
+        <v>195</v>
+      </c>
+      <c r="I15">
+        <v>1951</v>
+      </c>
+      <c r="J15">
+        <v>76</v>
+      </c>
+      <c r="K15">
+        <f>(I15*J15)/$H$8</f>
+        <v>5.203579575364099</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>197</v>
+      </c>
+      <c r="H16" t="s">
+        <v>196</v>
+      </c>
+      <c r="I16">
+        <v>385</v>
+      </c>
+      <c r="J16">
+        <v>233</v>
+      </c>
+      <c r="K16">
+        <f>(I16*J16)/$H$8</f>
+        <v>3.1480961572205648</v>
+      </c>
+    </row>
+    <row r="17" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>199</v>
+      </c>
+      <c r="H17" t="s">
+        <v>198</v>
+      </c>
+      <c r="I17">
+        <v>368</v>
+      </c>
+      <c r="J17">
+        <v>173</v>
+      </c>
+      <c r="K17">
+        <f>(I17*J17)/$H$8</f>
+        <v>2.2342165292156517</v>
+      </c>
+    </row>
+    <row r="18" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>177</v>
+      </c>
+      <c r="H18" t="s">
+        <v>189</v>
+      </c>
+      <c r="I18">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G21" t="s">
+        <v>201</v>
+      </c>
+      <c r="H21">
+        <v>10523</v>
+      </c>
+    </row>
+    <row r="22" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G22" t="s">
+        <v>137</v>
+      </c>
+      <c r="H22" t="s">
+        <v>138</v>
+      </c>
+      <c r="I22" t="s">
+        <v>178</v>
+      </c>
+      <c r="J22" t="s">
+        <v>179</v>
+      </c>
+      <c r="K22" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="23" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G23" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="H23" t="s">
+        <v>187</v>
+      </c>
+      <c r="I23">
+        <v>2086</v>
+      </c>
+      <c r="J23">
+        <v>19</v>
+      </c>
+      <c r="K23">
+        <f>(I23*J23)/$H$21</f>
+        <v>3.7664164211726692</v>
+      </c>
+    </row>
+    <row r="24" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G24" t="s">
+        <v>191</v>
+      </c>
+      <c r="H24" t="s">
+        <v>190</v>
+      </c>
+      <c r="I24">
+        <v>1784</v>
+      </c>
+      <c r="J24">
+        <v>38</v>
+      </c>
+      <c r="K24">
+        <f t="shared" ref="K24:K29" si="0">(I24*J24)/$H$21</f>
+        <v>6.4422693148341725</v>
+      </c>
+    </row>
+    <row r="25" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G25" t="s">
+        <v>184</v>
+      </c>
+      <c r="H25" t="s">
+        <v>192</v>
+      </c>
+      <c r="I25">
+        <v>254</v>
+      </c>
+      <c r="J25">
+        <v>104</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="0"/>
+        <v>2.5103107478855842</v>
+      </c>
+    </row>
+    <row r="26" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G26" t="s">
+        <v>185</v>
+      </c>
+      <c r="H26" t="s">
+        <v>193</v>
+      </c>
+      <c r="I26">
+        <v>483</v>
+      </c>
+      <c r="J26">
+        <v>72</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="0"/>
+        <v>3.3047609997149103</v>
+      </c>
+    </row>
+    <row r="27" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G27" t="s">
+        <v>194</v>
+      </c>
+      <c r="H27" t="s">
+        <v>195</v>
+      </c>
+      <c r="I27">
+        <v>667</v>
+      </c>
+      <c r="J27">
+        <v>38</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="0"/>
+        <v>2.4086287180461845</v>
+      </c>
+    </row>
+    <row r="28" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G28" t="s">
+        <v>197</v>
+      </c>
+      <c r="H28" t="s">
+        <v>196</v>
+      </c>
+      <c r="I28">
+        <v>181</v>
+      </c>
+      <c r="J28">
+        <v>175</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="0"/>
+        <v>3.0100731730495105</v>
+      </c>
+    </row>
+    <row r="29" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G29" t="s">
+        <v>199</v>
+      </c>
+      <c r="H29" t="s">
+        <v>198</v>
+      </c>
+      <c r="I29">
+        <v>264</v>
+      </c>
+      <c r="J29">
+        <v>79</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="0"/>
+        <v>1.9819443124584244</v>
+      </c>
+    </row>
+    <row r="30" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G30" t="s">
+        <v>177</v>
+      </c>
+      <c r="H30" t="s">
+        <v>189</v>
+      </c>
+      <c r="I30">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
@@ -3682,7 +4215,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
@@ -3976,7 +4509,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
@@ -4210,7 +4743,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update questions after meeting with Prof. Webb
</commit_message>
<xml_diff>
--- a/File/Lattice.xlsx
+++ b/File/Lattice.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3280" yWindow="920" windowWidth="19760" windowHeight="14020" tabRatio="500" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="1940" yWindow="1920" windowWidth="20040" windowHeight="12720" tabRatio="500" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="201">
   <si>
     <t>null</t>
   </si>
@@ -804,9 +804,6 @@
     <t>field1 = Age41-50 &amp; field4 = EduNum15 &amp; field2 = Self-emp-inc</t>
   </si>
   <si>
-    <t>field6 = Exec-managerial (Exclusive domain)</t>
-  </si>
-  <si>
     <t>&gt;50K &amp; field1 = Age41-50 &amp; field4 = EduNum15 &amp; field2 = Self-emp-inc &amp; edom()</t>
   </si>
   <si>
@@ -843,7 +840,7 @@
     <t>Itemset</t>
   </si>
   <si>
-    <t>field10 = Hour36-50 (Exclusive domain)</t>
+    <t>field6 != Exec-managerial AND field10 != Hour36-50 (Exclusive domain)</t>
   </si>
 </sst>
 </file>
@@ -1228,7 +1225,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2616200</xdr:colOff>
+      <xdr:colOff>3200400</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>134878</xdr:rowOff>
     </xdr:to>
@@ -3355,18 +3352,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="7.83203125" customWidth="1"/>
-    <col min="7" max="7" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="52.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.83203125" customWidth="1"/>
+    <col min="8" max="8" width="72.1640625" customWidth="1"/>
     <col min="9" max="10" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -3429,10 +3426,10 @@
         <v>1.7689874389607198E-2</v>
       </c>
       <c r="G8" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="H8">
-        <v>28495</v>
+        <v>9406</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -3470,32 +3467,32 @@
         <v>187</v>
       </c>
       <c r="I11">
-        <v>5873</v>
+        <v>1537</v>
       </c>
       <c r="J11">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="K11">
-        <f>(I11*J11)/$H$8</f>
-        <v>7.0076153711177396</v>
+        <f t="shared" ref="K11:K17" si="0">(I11*J11)/$H$8</f>
+        <v>2.941314054858601</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I12">
-        <v>5794</v>
+        <v>1491</v>
       </c>
       <c r="J12">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="K12">
-        <f>(I12*J12)/$H$8</f>
-        <v>15.046709949113879</v>
+        <f t="shared" si="0"/>
+        <v>5.865086115245588</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -3503,38 +3500,38 @@
         <v>184</v>
       </c>
       <c r="H13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I13">
-        <v>524</v>
+        <v>236</v>
       </c>
       <c r="J13">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="K13">
-        <f>(I13*J13)/$H$8</f>
-        <v>2.482540796630988</v>
+        <f t="shared" si="0"/>
+        <v>1.7814161173718903</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G14" t="s">
         <v>185</v>
       </c>
       <c r="H14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I14">
-        <v>716</v>
+        <v>326</v>
       </c>
       <c r="J14">
-        <v>150</v>
+        <v>65</v>
       </c>
       <c r="K14">
-        <f>(I14*J14)/$H$8</f>
-        <v>3.7690822951394982</v>
+        <f t="shared" si="0"/>
+        <v>2.2528173506272591</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -3542,56 +3539,56 @@
         <v>186</v>
       </c>
       <c r="G15" t="s">
+        <v>193</v>
+      </c>
+      <c r="H15" t="s">
         <v>194</v>
       </c>
-      <c r="H15" t="s">
-        <v>195</v>
-      </c>
       <c r="I15">
-        <v>1951</v>
+        <v>490</v>
       </c>
       <c r="J15">
-        <v>76</v>
+        <v>37</v>
       </c>
       <c r="K15">
-        <f>(I15*J15)/$H$8</f>
-        <v>5.203579575364099</v>
+        <f t="shared" si="0"/>
+        <v>1.9274930895173294</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H16" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I16">
-        <v>385</v>
+        <v>167</v>
       </c>
       <c r="J16">
-        <v>233</v>
+        <v>123</v>
       </c>
       <c r="K16">
-        <f>(I16*J16)/$H$8</f>
-        <v>3.1480961572205648</v>
+        <f t="shared" si="0"/>
+        <v>2.1838188390389113</v>
       </c>
     </row>
     <row r="17" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H17" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I17">
-        <v>368</v>
+        <v>165</v>
       </c>
       <c r="J17">
-        <v>173</v>
+        <v>72</v>
       </c>
       <c r="K17">
-        <f>(I17*J17)/$H$8</f>
-        <v>2.2342165292156517</v>
+        <f t="shared" si="0"/>
+        <v>1.2630236019561982</v>
       </c>
     </row>
     <row r="18" spans="7:11" x14ac:dyDescent="0.2">
@@ -3599,173 +3596,14 @@
         <v>177</v>
       </c>
       <c r="H18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I18">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="G21" t="s">
-        <v>201</v>
-      </c>
-      <c r="H21">
-        <v>10523</v>
-      </c>
-    </row>
-    <row r="22" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="G22" t="s">
-        <v>137</v>
-      </c>
-      <c r="H22" t="s">
-        <v>138</v>
-      </c>
-      <c r="I22" t="s">
-        <v>178</v>
-      </c>
-      <c r="J22" t="s">
-        <v>179</v>
-      </c>
-      <c r="K22" t="s">
-        <v>180</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="G23" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="H23" t="s">
-        <v>187</v>
-      </c>
-      <c r="I23">
-        <v>2086</v>
-      </c>
-      <c r="J23">
-        <v>19</v>
-      </c>
-      <c r="K23">
-        <f>(I23*J23)/$H$21</f>
-        <v>3.7664164211726692</v>
-      </c>
-    </row>
-    <row r="24" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="G24" t="s">
-        <v>191</v>
-      </c>
-      <c r="H24" t="s">
-        <v>190</v>
-      </c>
-      <c r="I24">
-        <v>1784</v>
-      </c>
-      <c r="J24">
-        <v>38</v>
-      </c>
-      <c r="K24">
-        <f t="shared" ref="K24:K29" si="0">(I24*J24)/$H$21</f>
-        <v>6.4422693148341725</v>
-      </c>
-    </row>
-    <row r="25" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="G25" t="s">
-        <v>184</v>
-      </c>
-      <c r="H25" t="s">
-        <v>192</v>
-      </c>
-      <c r="I25">
-        <v>254</v>
-      </c>
-      <c r="J25">
-        <v>104</v>
-      </c>
-      <c r="K25">
-        <f t="shared" si="0"/>
-        <v>2.5103107478855842</v>
-      </c>
-    </row>
-    <row r="26" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="G26" t="s">
-        <v>185</v>
-      </c>
-      <c r="H26" t="s">
-        <v>193</v>
-      </c>
-      <c r="I26">
-        <v>483</v>
-      </c>
-      <c r="J26">
-        <v>72</v>
-      </c>
-      <c r="K26">
-        <f t="shared" si="0"/>
-        <v>3.3047609997149103</v>
-      </c>
-    </row>
-    <row r="27" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="G27" t="s">
-        <v>194</v>
-      </c>
-      <c r="H27" t="s">
-        <v>195</v>
-      </c>
-      <c r="I27">
-        <v>667</v>
-      </c>
-      <c r="J27">
-        <v>38</v>
-      </c>
-      <c r="K27">
-        <f t="shared" si="0"/>
-        <v>2.4086287180461845</v>
-      </c>
-    </row>
-    <row r="28" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="G28" t="s">
-        <v>197</v>
-      </c>
-      <c r="H28" t="s">
-        <v>196</v>
-      </c>
-      <c r="I28">
-        <v>181</v>
-      </c>
-      <c r="J28">
-        <v>175</v>
-      </c>
-      <c r="K28">
-        <f t="shared" si="0"/>
-        <v>3.0100731730495105</v>
-      </c>
-    </row>
-    <row r="29" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="G29" t="s">
-        <v>199</v>
-      </c>
-      <c r="H29" t="s">
-        <v>198</v>
-      </c>
-      <c r="I29">
-        <v>264</v>
-      </c>
-      <c r="J29">
-        <v>79</v>
-      </c>
-      <c r="K29">
-        <f t="shared" si="0"/>
-        <v>1.9819443124584244</v>
-      </c>
-    </row>
-    <row r="30" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="G30" t="s">
-        <v>177</v>
-      </c>
-      <c r="H30" t="s">
-        <v>189</v>
-      </c>
-      <c r="I30">
-        <v>19</v>
-      </c>
+      <c r="G23" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>